<commit_message>
All solvents 1 figure
</commit_message>
<xml_diff>
--- a/Heatmap CSV/Combined Ext TIS LOO.xlsx
+++ b/Heatmap CSV/Combined Ext TIS LOO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeffreyvanhumbeck/Documents/GitHub/Bitumen-ML/Heatmap CSV/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{25CC9D7B-E125-A540-A450-74DCFE8D9868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70FCBDA9-B821-5C4F-906C-3E0DDC87B624}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="620" windowWidth="34560" windowHeight="19500" xr2:uid="{BDAA7132-29C0-B548-B94C-8B5BE4F97458}"/>
   </bookViews>
@@ -354,7 +354,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -373,6 +373,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -386,7 +392,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -396,6 +402,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -716,7 +724,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A33" sqref="A33:XFD33"/>
+      <selection pane="bottomRight" activeCell="O36" sqref="O36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -931,7 +939,7 @@
       <c r="N2" s="3">
         <v>2.7335E-4</v>
       </c>
-      <c r="O2" s="3">
+      <c r="O2" s="9">
         <v>2.4121E-4</v>
       </c>
       <c r="P2" s="3">
@@ -1118,7 +1126,7 @@
       <c r="N3" s="3">
         <v>2.1965E-4</v>
       </c>
-      <c r="O3" s="3">
+      <c r="O3" s="9">
         <v>2.3018E-4</v>
       </c>
       <c r="P3" s="3">
@@ -1305,7 +1313,7 @@
       <c r="N4">
         <v>6.2288999999999997E-4</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="7">
         <v>5.6433999999999998E-4</v>
       </c>
       <c r="P4">
@@ -1492,7 +1500,7 @@
       <c r="N5">
         <v>3.6212000000000001E-4</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="10">
         <v>3.7731E-4</v>
       </c>
       <c r="P5">
@@ -1679,7 +1687,7 @@
       <c r="N6">
         <v>2.4196999999999999E-4</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="10">
         <v>2.4549000000000001E-4</v>
       </c>
       <c r="P6">
@@ -1866,7 +1874,7 @@
       <c r="N7" s="3">
         <v>2.4101E-4</v>
       </c>
-      <c r="O7" s="3">
+      <c r="O7" s="9">
         <v>2.3269E-4</v>
       </c>
       <c r="P7" s="3">
@@ -2053,7 +2061,7 @@
       <c r="N8" s="3">
         <v>2.0325999999999999E-3</v>
       </c>
-      <c r="O8" s="3">
+      <c r="O8" s="8">
         <v>1.9161E-3</v>
       </c>
       <c r="P8" s="3">
@@ -2240,7 +2248,7 @@
       <c r="N9">
         <v>5.3390000000000002E-4</v>
       </c>
-      <c r="O9">
+      <c r="O9" s="10">
         <v>3.7754999999999999E-4</v>
       </c>
       <c r="P9">
@@ -2427,7 +2435,7 @@
       <c r="N10" s="3">
         <v>3.9510000000000001E-4</v>
       </c>
-      <c r="O10" s="3">
+      <c r="O10" s="9">
         <v>3.0662000000000002E-4</v>
       </c>
       <c r="P10" s="3">
@@ -2614,7 +2622,7 @@
       <c r="N11" s="3">
         <v>4.5176999999999999E-4</v>
       </c>
-      <c r="O11" s="3">
+      <c r="O11" s="9">
         <v>5.4350999999999998E-4</v>
       </c>
       <c r="P11" s="3">
@@ -2801,7 +2809,7 @@
       <c r="N12" s="3">
         <v>1.8822000000000001E-3</v>
       </c>
-      <c r="O12" s="3">
+      <c r="O12" s="8">
         <v>1.8749000000000001E-3</v>
       </c>
       <c r="P12" s="3">
@@ -2988,7 +2996,7 @@
       <c r="N13" s="3">
         <v>5.1266999999999997E-3</v>
       </c>
-      <c r="O13" s="3">
+      <c r="O13" s="9">
         <v>5.0618E-3</v>
       </c>
       <c r="P13" s="3">
@@ -3175,7 +3183,7 @@
       <c r="N14" s="3">
         <v>8.6932000000000003E-4</v>
       </c>
-      <c r="O14" s="3">
+      <c r="O14" s="9">
         <v>7.5516999999999999E-4</v>
       </c>
       <c r="P14" s="3">
@@ -3362,7 +3370,7 @@
       <c r="N15" s="3">
         <v>7.3930000000000003E-4</v>
       </c>
-      <c r="O15" s="3">
+      <c r="O15" s="9">
         <v>7.0171000000000003E-4</v>
       </c>
       <c r="P15" s="3">
@@ -3549,7 +3557,7 @@
       <c r="N16" s="3">
         <v>2.7190999999999999E-3</v>
       </c>
-      <c r="O16" s="3">
+      <c r="O16" s="9">
         <v>2.5093000000000001E-4</v>
       </c>
       <c r="P16" s="3">
@@ -3736,7 +3744,7 @@
       <c r="N17">
         <v>1.0042E-3</v>
       </c>
-      <c r="O17">
+      <c r="O17" s="10">
         <v>9.8951000000000009E-4</v>
       </c>
       <c r="P17">
@@ -3923,7 +3931,7 @@
       <c r="N18" s="3">
         <v>4.0026999999999999E-4</v>
       </c>
-      <c r="O18" s="3">
+      <c r="O18" s="9">
         <v>3.7364000000000001E-4</v>
       </c>
       <c r="P18" s="3">
@@ -4110,7 +4118,7 @@
       <c r="N19" s="3">
         <v>3.0200000000000002E-4</v>
       </c>
-      <c r="O19" s="3">
+      <c r="O19" s="9">
         <v>3.0066000000000001E-4</v>
       </c>
       <c r="P19" s="3">
@@ -4297,7 +4305,7 @@
       <c r="N20" s="3">
         <v>3.7624099999999999E-3</v>
       </c>
-      <c r="O20" s="3">
+      <c r="O20" s="9">
         <v>1.5018E-3</v>
       </c>
       <c r="P20" s="3">
@@ -4484,7 +4492,7 @@
       <c r="N21">
         <v>2.4782300000000001E-3</v>
       </c>
-      <c r="O21">
+      <c r="O21" s="10">
         <v>2.5834999999999999E-3</v>
       </c>
       <c r="P21">
@@ -4671,7 +4679,7 @@
       <c r="N22">
         <v>5.3939199999999997E-4</v>
       </c>
-      <c r="O22">
+      <c r="O22" s="10">
         <v>6.3701000000000003E-4</v>
       </c>
       <c r="P22">
@@ -4858,7 +4866,7 @@
       <c r="N23">
         <v>9.6002000000000001E-4</v>
       </c>
-      <c r="O23">
+      <c r="O23" s="10">
         <v>1.0152E-3</v>
       </c>
       <c r="P23">
@@ -5045,7 +5053,7 @@
       <c r="N24">
         <v>4.4752999999999998E-3</v>
       </c>
-      <c r="O24">
+      <c r="O24" s="10">
         <v>2.1638999999999999E-3</v>
       </c>
       <c r="P24">
@@ -5232,7 +5240,7 @@
       <c r="N25">
         <v>2.5221E-4</v>
       </c>
-      <c r="O25">
+      <c r="O25" s="10">
         <v>2.4783999999999999E-4</v>
       </c>
       <c r="P25">
@@ -5419,7 +5427,7 @@
       <c r="N26">
         <v>2.54231E-4</v>
       </c>
-      <c r="O26">
+      <c r="O26" s="10">
         <v>2.498E-4</v>
       </c>
       <c r="P26">
@@ -5606,7 +5614,7 @@
       <c r="N27" s="3">
         <v>3.0446E-4</v>
       </c>
-      <c r="O27" s="3">
+      <c r="O27" s="9">
         <v>2.9845000000000002E-4</v>
       </c>
       <c r="P27" s="3">
@@ -5793,7 +5801,7 @@
       <c r="N28" s="3">
         <v>4.1315999999999998E-4</v>
       </c>
-      <c r="O28" s="3">
+      <c r="O28" s="8">
         <v>3.8963000000000002E-4</v>
       </c>
       <c r="P28" s="3">
@@ -5980,7 +5988,7 @@
       <c r="N29" s="3">
         <v>4.4495E-4</v>
       </c>
-      <c r="O29" s="3">
+      <c r="O29" s="9">
         <v>6.1326999999999996E-4</v>
       </c>
       <c r="P29" s="3">
@@ -6167,7 +6175,7 @@
       <c r="N30" s="3">
         <v>1.256E-3</v>
       </c>
-      <c r="O30" s="3">
+      <c r="O30" s="9">
         <v>1.1872E-3</v>
       </c>
       <c r="P30" s="3">
@@ -6354,7 +6362,7 @@
       <c r="N31" s="3">
         <v>2.9479000000000002E-4</v>
       </c>
-      <c r="O31" s="3">
+      <c r="O31" s="9">
         <v>2.6988000000000001E-4</v>
       </c>
       <c r="P31" s="3">
@@ -6541,7 +6549,7 @@
       <c r="N32" s="3">
         <v>3.3024999999999998E-4</v>
       </c>
-      <c r="O32" s="3">
+      <c r="O32" s="9">
         <v>3.5163000000000002E-4</v>
       </c>
       <c r="P32" s="3">
@@ -6728,7 +6736,7 @@
       <c r="N33" s="3">
         <v>1.1316E-3</v>
       </c>
-      <c r="O33" s="3">
+      <c r="O33" s="9">
         <v>8.6300999999999999E-4</v>
       </c>
       <c r="P33" s="3">
@@ -6915,7 +6923,7 @@
       <c r="N34" s="3">
         <v>3.8420000000000001E-4</v>
       </c>
-      <c r="O34" s="3">
+      <c r="O34" s="9">
         <v>3.8162999999999999E-4</v>
       </c>
       <c r="P34" s="3">
@@ -7102,7 +7110,7 @@
       <c r="N35" s="3">
         <v>3.8666999999999998E-4</v>
       </c>
-      <c r="O35" s="3">
+      <c r="O35" s="8">
         <v>3.9365E-4</v>
       </c>
       <c r="P35" s="3">
@@ -7289,7 +7297,7 @@
       <c r="N36" s="3">
         <v>5.6811000000000003E-4</v>
       </c>
-      <c r="O36" s="3">
+      <c r="O36" s="9">
         <v>5.8303999999999995E-4</v>
       </c>
       <c r="P36" s="3">

</xml_diff>